<commit_message>
changes done 1 Feb 2024
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testData.xlsx
+++ b/src/test/resources/testData/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13770" windowHeight="6180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16785" windowHeight="6180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="loginCredentials" sheetId="4" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="Coverages" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M18"/>
+  <oleSize ref="A1:J18"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -305,13 +305,13 @@
     <t>Coverage</t>
   </si>
   <si>
-    <t>Policy_30012024_</t>
-  </si>
-  <si>
-    <t>Report_30012024_</t>
-  </si>
-  <si>
     <t>user.quick</t>
+  </si>
+  <si>
+    <t>Policy_01022024_</t>
+  </si>
+  <si>
+    <t>Report_01022024_</t>
   </si>
 </sst>
 </file>
@@ -732,7 +732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -761,7 +761,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>3</v>
@@ -780,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,7 +808,7 @@
         <v>85</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C2" s="5">
         <v>2</v>
@@ -841,7 +841,7 @@
         <v>90</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C5" s="5">
         <v>5</v>

</xml_diff>